<commit_message>
Included objects for ActionRequired and ActionOverdue Count.
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FULPP_WS\Fulcrum_PreProd_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreProdWS\Fulcrum_PreProd_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="Objects" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Objects_Navigation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t>textbox</t>
   </si>
@@ -257,12 +257,24 @@
   </si>
   <si>
     <t>New Mail</t>
+  </si>
+  <si>
+    <t>.//*[@class='action-number action-required-number']</t>
+  </si>
+  <si>
+    <t>Usersite Menu - Action Required Count</t>
+  </si>
+  <si>
+    <t>Usersite Menu - Actions Overdue Count</t>
+  </si>
+  <si>
+    <t>.//*[@class='action-number action-overdue-number']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -895,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1028,50 +1040,50 @@
         <v>76</v>
       </c>
     </row>
+    <row r="9" spans="1:9">
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5" t="s">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>52</v>
-      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -1080,139 +1092,167 @@
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="5" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="B17" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="B20" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>34</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>9</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
+    <row r="24" spans="1:7">
+      <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="B23" t="s">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
         <v>9</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="5" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="B26" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" t="s">
         <v>67</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E28" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A24:G24"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20 C23 C17:C18 C3:C9 C11:C15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C25 C19:C20 C13:C17 C3:C11">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1226,7 +1266,7 @@
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$40</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:D15 D17:D18 D3:D9 D20:D21 D23:D24 D26</xm:sqref>
+          <xm:sqref>D13:D17 D19:D20 D28 D22:D23 D25:D26 D3:D11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added User Site Setting wheel navigation section
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Navigation.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreProdWS\Fulcrum_PreProd_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fulcrum_Preprod\Fulcrum_PreProd_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>textbox</t>
   </si>
@@ -269,6 +269,27 @@
   </si>
   <si>
     <t>.//*[@class='action-number action-overdue-number']</t>
+  </si>
+  <si>
+    <t>User Site Setting wheel navigation</t>
+  </si>
+  <si>
+    <t>Settings Wheel</t>
+  </si>
+  <si>
+    <t>.//*[@id='siteactiontd']</t>
+  </si>
+  <si>
+    <t>Site contents</t>
+  </si>
+  <si>
+    <t>//*[ text()='Site contents']</t>
+  </si>
+  <si>
+    <t>add an app</t>
+  </si>
+  <si>
+    <t>.//*[@id='apptile-appadd']/div[1]/a</t>
   </si>
 </sst>
 </file>
@@ -907,10 +928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1242,8 +1263,62 @@
         <v>74</v>
       </c>
     </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A30:G30"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A12:G12"/>
@@ -1251,8 +1326,11 @@
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="A24:G24"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C22 C25 C19:C20 C13:C17 C3:C11">
+      <formula1>"id,name,xpath"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C33">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1261,13 +1339,19 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$40</xm:f>
           </x14:formula1>
           <xm:sqref>D13:D17 D19:D20 D28 D22:D23 D25:D26 D3:D11</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Objects!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D31:D33</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>